<commit_message>
fixing issue with creating df_parameters
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E56A4EC-4A00-46DE-A350-5243B3DE3CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1318ACA-6966-4CB6-AD73-ED7F1AAAFEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="300" windowWidth="37200" windowHeight="20700" activeTab="5" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -894,15 +894,15 @@
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.26171875" customWidth="1"/>
+    <col min="10" max="10" width="4.41796875" customWidth="1"/>
+    <col min="11" max="11" width="9.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -914,7 +914,7 @@
       <c r="J2" s="19"/>
       <c r="K2" s="20"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="21"/>
       <c r="C3" s="22" t="s">
         <v>10</v>
@@ -928,7 +928,7 @@
       <c r="J3" s="23"/>
       <c r="K3" s="24"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="21"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -940,7 +940,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="21"/>
       <c r="C5" s="23" t="s">
         <v>16</v>
@@ -954,7 +954,7 @@
       <c r="J5" s="23"/>
       <c r="K5" s="24"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="21"/>
       <c r="C6" s="23" t="s">
         <v>14</v>
@@ -968,7 +968,7 @@
       <c r="J6" s="23"/>
       <c r="K6" s="24"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="21"/>
       <c r="C7" s="23" t="s">
         <v>11</v>
@@ -982,7 +982,7 @@
       <c r="J7" s="23"/>
       <c r="K7" s="24"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="21"/>
       <c r="C8" s="23" t="s">
         <v>12</v>
@@ -996,7 +996,7 @@
       <c r="J8" s="23"/>
       <c r="K8" s="24"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="21"/>
       <c r="C9" s="23" t="s">
         <v>13</v>
@@ -1010,7 +1010,7 @@
       <c r="J9" s="23"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="21"/>
       <c r="C10" s="23" t="s">
         <v>52</v>
@@ -1024,7 +1024,7 @@
       <c r="J10" s="23"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="21"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -1036,7 +1036,7 @@
       <c r="J11" s="23"/>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="21"/>
       <c r="C12" s="23" t="s">
         <v>17</v>
@@ -1050,7 +1050,7 @@
       <c r="J12" s="23"/>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="21"/>
       <c r="C13" s="23" t="s">
         <v>15</v>
@@ -1064,7 +1064,7 @@
       <c r="J13" s="23"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="21"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -1076,7 +1076,7 @@
       <c r="J14" s="23"/>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="21"/>
       <c r="C15" s="23" t="s">
         <v>18</v>
@@ -1090,7 +1090,7 @@
       <c r="J15" s="23"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="21"/>
       <c r="C16" s="23" t="s">
         <v>19</v>
@@ -1104,7 +1104,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="21"/>
       <c r="C17" s="23" t="s">
         <v>20</v>
@@ -1118,7 +1118,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="21"/>
       <c r="C18" s="23" t="s">
         <v>21</v>
@@ -1132,7 +1132,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="21"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -1144,7 +1144,7 @@
       <c r="J19" s="23"/>
       <c r="K19" s="24"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="21"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -1156,7 +1156,7 @@
       <c r="J20" s="23"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="21"/>
       <c r="C21" s="25" t="s">
         <v>22</v>
@@ -1172,7 +1172,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="21"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -1184,7 +1184,7 @@
       <c r="J22" s="23"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="21"/>
       <c r="C23" s="26" t="s">
         <v>24</v>
@@ -1200,7 +1200,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="21"/>
       <c r="C24" s="26" t="s">
         <v>25</v>
@@ -1216,7 +1216,7 @@
       <c r="J24" s="23"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="21"/>
       <c r="C25" s="26" t="s">
         <v>26</v>
@@ -1232,7 +1232,7 @@
       <c r="J25" s="23"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="21"/>
       <c r="C26" s="26" t="s">
         <v>30</v>
@@ -1248,7 +1248,7 @@
       <c r="J26" s="23"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="21"/>
       <c r="C27" s="26" t="s">
         <v>32</v>
@@ -1264,7 +1264,7 @@
       <c r="J27" s="23"/>
       <c r="K27" s="24"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="21"/>
       <c r="C28" s="26" t="s">
         <v>34</v>
@@ -1280,7 +1280,7 @@
       <c r="J28" s="23"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="21"/>
       <c r="C29" s="26" t="s">
         <v>35</v>
@@ -1296,7 +1296,7 @@
       <c r="J29" s="23"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="21"/>
       <c r="C30" s="26" t="s">
         <v>38</v>
@@ -1312,7 +1312,7 @@
       <c r="J30" s="23"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="21"/>
       <c r="C31" s="26" t="s">
         <v>40</v>
@@ -1331,7 +1331,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="21"/>
       <c r="C32" s="26" t="s">
         <v>43</v>
@@ -1347,7 +1347,7 @@
       <c r="J32" s="23"/>
       <c r="K32" s="24"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="21"/>
       <c r="C33" s="26" t="s">
         <v>42</v>
@@ -1363,7 +1363,7 @@
       <c r="J33" s="23"/>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="21"/>
       <c r="C34" s="26" t="s">
         <v>46</v>
@@ -1379,7 +1379,7 @@
       <c r="J34" s="23"/>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="21"/>
       <c r="C35" s="26" t="s">
         <v>48</v>
@@ -1395,7 +1395,7 @@
       <c r="J35" s="23"/>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="21"/>
       <c r="C36" s="26" t="s">
         <v>49</v>
@@ -1411,7 +1411,7 @@
       <c r="J36" s="23"/>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -1450,27 +1450,27 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="2" width="9.26171875" style="1"/>
+    <col min="3" max="3" width="3.578125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.26171875" style="1"/>
+    <col min="13" max="13" width="11.26171875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1512,7 +1512,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +1533,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1586,34 +1586,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.26171875" style="1"/>
+    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1633,7 +1633,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1653,7 +1653,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1673,7 +1673,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1693,7 +1693,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1713,7 +1713,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1733,7 +1733,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1768,28 +1768,28 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.28515625" style="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="3" width="9.26171875" style="1"/>
+    <col min="4" max="4" width="4.41796875" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.26171875" style="1"/>
+    <col min="15" max="15" width="12.15625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>55</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1828,7 +1828,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1846,7 +1846,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1864,7 +1864,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1894,20 +1894,20 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9"/>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -1934,7 +1934,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1960,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
@@ -2025,7 +2025,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -2038,52 +2038,52 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -2098,21 +2098,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>57</v>
@@ -2130,7 +2130,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -2148,47 +2148,47 @@
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2208,17 +2208,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4"/>
       <c r="B2" s="7" t="s">
         <v>57</v>
@@ -2236,7 +2236,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2246,59 +2246,59 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>

</xml_diff>

<commit_message>
disposal constraint correction and data read-in
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -5,21 +5,40 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1318ACA-6966-4CB6-AD73-ED7F1AAAFEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43351AE-F7C4-49FD-8818-FC825D7D7ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="22" activeTab="24" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
     <sheet name="ProductionPads" sheetId="1" r:id="rId2"/>
-    <sheet name="CompletionsPads" sheetId="3" r:id="rId3"/>
-    <sheet name="SWDSites" sheetId="4" r:id="rId4"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId5"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId6"/>
-    <sheet name="FlowbackRates" sheetId="12" r:id="rId7"/>
+    <sheet name="ProductionTanks" sheetId="34" r:id="rId3"/>
+    <sheet name="CompletionsPads" sheetId="3" r:id="rId4"/>
+    <sheet name="SWDSites" sheetId="4" r:id="rId5"/>
+    <sheet name="FreshwaterSources" sheetId="35" r:id="rId6"/>
+    <sheet name="StorageSites" sheetId="36" r:id="rId7"/>
+    <sheet name="TreatmentSites" sheetId="37" r:id="rId8"/>
+    <sheet name="ReuseOptions" sheetId="38" r:id="rId9"/>
+    <sheet name="NetworkNodes" sheetId="39" r:id="rId10"/>
+    <sheet name="FCA" sheetId="41" r:id="rId11"/>
+    <sheet name="PCT" sheetId="42" r:id="rId12"/>
+    <sheet name="PKT" sheetId="43" r:id="rId13"/>
+    <sheet name="CKT" sheetId="44" r:id="rId14"/>
+    <sheet name="PAL" sheetId="45" r:id="rId15"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId16"/>
+    <sheet name="ProductionRates" sheetId="40" r:id="rId17"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId18"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId19"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId20"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId21"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId22"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId23"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId24"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId25"/>
+    <sheet name="FlowbackRates" sheetId="12" r:id="rId26"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="98">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -220,6 +239,111 @@
   </si>
   <si>
     <t>Table of Flowback Rates for Completion Pads over Weeks [bbl/day]</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>List of all Production Tank Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Freshwater Source Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Storage Site Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Treatment Site Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Reuse Option Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Network Node Identifiers [-]</t>
+  </si>
+  <si>
+    <t>Table of Production Rate Forecasts by Tanks and Pads [bbl/day]</t>
+  </si>
+  <si>
+    <t>Freshwater Sources to Completions Pads Piping Arcs [-]</t>
+  </si>
+  <si>
+    <t>Production Pads to Completions Pads Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>Production Pads to Disposal Sites Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>Completions Pads to Disposal Sites Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>Production Pads to Production Tanks Links [-]</t>
+  </si>
+  <si>
+    <t>Table of Initial Disposal Capacity  [bbl/day]</t>
+  </si>
+  <si>
+    <t>Table of Freshwater Sourcing Availability [bbl/day]</t>
+  </si>
+  <si>
+    <t>Table of Pad Offloading Capacity  [bbl/day]</t>
+  </si>
+  <si>
+    <t>Table of Disposal Operational Cost  [$/bbl]</t>
+  </si>
+  <si>
+    <t>Table of Reuse Operational Cost  [$/bbl]</t>
+  </si>
+  <si>
+    <t>Table of Trucking Hourly Cost  [$/hour]</t>
+  </si>
+  <si>
+    <t>Table of Freshwater Sourcing Cost  [$/hour]</t>
   </si>
 </sst>
 </file>
@@ -306,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -470,12 +594,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,6 +711,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -894,15 +1116,15 @@
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.26171875" customWidth="1"/>
-    <col min="10" max="10" width="4.41796875" customWidth="1"/>
-    <col min="11" max="11" width="9.41796875" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -914,7 +1136,7 @@
       <c r="J2" s="19"/>
       <c r="K2" s="20"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="21"/>
       <c r="C3" s="22" t="s">
         <v>10</v>
@@ -928,7 +1150,7 @@
       <c r="J3" s="23"/>
       <c r="K3" s="24"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="21"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -940,7 +1162,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
       <c r="C5" s="23" t="s">
         <v>16</v>
@@ -954,7 +1176,7 @@
       <c r="J5" s="23"/>
       <c r="K5" s="24"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="21"/>
       <c r="C6" s="23" t="s">
         <v>14</v>
@@ -968,7 +1190,7 @@
       <c r="J6" s="23"/>
       <c r="K6" s="24"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="23" t="s">
         <v>11</v>
@@ -982,7 +1204,7 @@
       <c r="J7" s="23"/>
       <c r="K7" s="24"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
       <c r="C8" s="23" t="s">
         <v>12</v>
@@ -996,7 +1218,7 @@
       <c r="J8" s="23"/>
       <c r="K8" s="24"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="23" t="s">
         <v>13</v>
@@ -1010,7 +1232,7 @@
       <c r="J9" s="23"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="23" t="s">
         <v>52</v>
@@ -1024,7 +1246,7 @@
       <c r="J10" s="23"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -1036,7 +1258,7 @@
       <c r="J11" s="23"/>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
       <c r="C12" s="23" t="s">
         <v>17</v>
@@ -1050,7 +1272,7 @@
       <c r="J12" s="23"/>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="23" t="s">
         <v>15</v>
@@ -1064,7 +1286,7 @@
       <c r="J13" s="23"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -1076,7 +1298,7 @@
       <c r="J14" s="23"/>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="23" t="s">
         <v>18</v>
@@ -1090,7 +1312,7 @@
       <c r="J15" s="23"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="23" t="s">
         <v>19</v>
@@ -1104,7 +1326,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="23" t="s">
         <v>20</v>
@@ -1118,7 +1340,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="23" t="s">
         <v>21</v>
@@ -1132,7 +1354,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -1144,7 +1366,7 @@
       <c r="J19" s="23"/>
       <c r="K19" s="24"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -1156,7 +1378,7 @@
       <c r="J20" s="23"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="25" t="s">
         <v>22</v>
@@ -1172,7 +1394,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -1184,7 +1406,7 @@
       <c r="J22" s="23"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="26" t="s">
         <v>24</v>
@@ -1200,7 +1422,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="26" t="s">
         <v>25</v>
@@ -1216,7 +1438,7 @@
       <c r="J24" s="23"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="26" t="s">
         <v>26</v>
@@ -1232,7 +1454,7 @@
       <c r="J25" s="23"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="26" t="s">
         <v>30</v>
@@ -1248,7 +1470,7 @@
       <c r="J26" s="23"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="26" t="s">
         <v>32</v>
@@ -1264,7 +1486,7 @@
       <c r="J27" s="23"/>
       <c r="K27" s="24"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
       <c r="C28" s="26" t="s">
         <v>34</v>
@@ -1280,7 +1502,7 @@
       <c r="J28" s="23"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="21"/>
       <c r="C29" s="26" t="s">
         <v>35</v>
@@ -1296,7 +1518,7 @@
       <c r="J29" s="23"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="21"/>
       <c r="C30" s="26" t="s">
         <v>38</v>
@@ -1312,7 +1534,7 @@
       <c r="J30" s="23"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="21"/>
       <c r="C31" s="26" t="s">
         <v>40</v>
@@ -1331,7 +1553,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="21"/>
       <c r="C32" s="26" t="s">
         <v>43</v>
@@ -1347,7 +1569,7 @@
       <c r="J32" s="23"/>
       <c r="K32" s="24"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="21"/>
       <c r="C33" s="26" t="s">
         <v>42</v>
@@ -1363,7 +1585,7 @@
       <c r="J33" s="23"/>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="21"/>
       <c r="C34" s="26" t="s">
         <v>46</v>
@@ -1379,7 +1601,7 @@
       <c r="J34" s="23"/>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="21"/>
       <c r="C35" s="26" t="s">
         <v>48</v>
@@ -1395,7 +1617,7 @@
       <c r="J35" s="23"/>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="21"/>
       <c r="C36" s="26" t="s">
         <v>49</v>
@@ -1411,7 +1633,7 @@
       <c r="J36" s="23"/>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -1445,175 +1667,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
-  <dimension ref="A1:R6"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.26171875" style="1"/>
-    <col min="3" max="3" width="3.578125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.26171875" style="1"/>
-    <col min="13" max="13" width="11.26171875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83984375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.578125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1633,7 +1717,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1653,7 +1737,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1673,7 +1757,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1693,7 +1777,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1713,7 +1797,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1733,7 +1817,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1754,44 +1838,1174 @@
       <c r="T9" s="2"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB6341-94DE-401B-89F3-66EA9EB6DBB9}">
-  <dimension ref="A1:R7"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="4.41796875" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.26171875" style="1"/>
-    <col min="15" max="15" width="12.15625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40"/>
+    </row>
+    <row r="4" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="42"/>
+      <c r="C7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABD83BE-FC18-4B07-A835-FE113535C483}">
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="40"/>
+    </row>
+    <row r="4" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="40"/>
+    </row>
+    <row r="5" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="40"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13">
+        <v>1</v>
+      </c>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6" s="13">
+        <v>1</v>
+      </c>
+      <c r="N6" s="13"/>
+      <c r="O6" s="40"/>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14">
+        <v>1</v>
+      </c>
+      <c r="O7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="14">
+        <v>31500</v>
+      </c>
+      <c r="C3" s="14">
+        <v>35000</v>
+      </c>
+      <c r="D3" s="14">
+        <v>35000</v>
+      </c>
+      <c r="E3" s="14">
+        <v>28000</v>
+      </c>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="12"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1058</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1029</v>
+      </c>
+      <c r="E3" s="13">
+        <v>999</v>
+      </c>
+      <c r="F3" s="13">
+        <v>998</v>
+      </c>
+      <c r="G3" s="40">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1058</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1029</v>
+      </c>
+      <c r="E4" s="13">
+        <v>999</v>
+      </c>
+      <c r="F4" s="13">
+        <v>998</v>
+      </c>
+      <c r="G4" s="40">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="13">
+        <v>466</v>
+      </c>
+      <c r="D5" s="13">
+        <v>460</v>
+      </c>
+      <c r="E5" s="13">
+        <v>458</v>
+      </c>
+      <c r="F5" s="13">
+        <v>457</v>
+      </c>
+      <c r="G5" s="40">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="13">
+        <v>466</v>
+      </c>
+      <c r="D6" s="13">
+        <v>460</v>
+      </c>
+      <c r="E6" s="13">
+        <v>458</v>
+      </c>
+      <c r="F6" s="13">
+        <v>457</v>
+      </c>
+      <c r="G6" s="40">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="13">
+        <v>466</v>
+      </c>
+      <c r="D7" s="13">
+        <v>460</v>
+      </c>
+      <c r="E7" s="13">
+        <v>458</v>
+      </c>
+      <c r="F7" s="13">
+        <v>457</v>
+      </c>
+      <c r="G7" s="40">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="13">
+        <v>200</v>
+      </c>
+      <c r="D8" s="13">
+        <v>199</v>
+      </c>
+      <c r="E8" s="13">
+        <v>198</v>
+      </c>
+      <c r="F8" s="13">
+        <v>196</v>
+      </c>
+      <c r="G8" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="13">
+        <v>200</v>
+      </c>
+      <c r="D9" s="13">
+        <v>199</v>
+      </c>
+      <c r="E9" s="13">
+        <v>198</v>
+      </c>
+      <c r="F9" s="13">
+        <v>196</v>
+      </c>
+      <c r="G9" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="13">
+        <v>200</v>
+      </c>
+      <c r="D10" s="13">
+        <v>199</v>
+      </c>
+      <c r="E10" s="13">
+        <v>198</v>
+      </c>
+      <c r="F10" s="13">
+        <v>196</v>
+      </c>
+      <c r="G10" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="13">
+        <v>200</v>
+      </c>
+      <c r="D11" s="13">
+        <v>199</v>
+      </c>
+      <c r="E11" s="13">
+        <v>198</v>
+      </c>
+      <c r="F11" s="13">
+        <v>196</v>
+      </c>
+      <c r="G11" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="13">
+        <v>331</v>
+      </c>
+      <c r="D12" s="13">
+        <v>330</v>
+      </c>
+      <c r="E12" s="13">
+        <v>330</v>
+      </c>
+      <c r="F12" s="13">
+        <v>329</v>
+      </c>
+      <c r="G12" s="40">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="13">
+        <v>331</v>
+      </c>
+      <c r="D13" s="13">
+        <v>330</v>
+      </c>
+      <c r="E13" s="13">
+        <v>330</v>
+      </c>
+      <c r="F13" s="13">
+        <v>329</v>
+      </c>
+      <c r="G13" s="40">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="13">
+        <v>331</v>
+      </c>
+      <c r="D14" s="13">
+        <v>330</v>
+      </c>
+      <c r="E14" s="13">
+        <v>330</v>
+      </c>
+      <c r="F14" s="13">
+        <v>329</v>
+      </c>
+      <c r="G14" s="40">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="13">
+        <v>895</v>
+      </c>
+      <c r="D15" s="13">
+        <v>888</v>
+      </c>
+      <c r="E15" s="13">
+        <v>887</v>
+      </c>
+      <c r="F15" s="13">
+        <v>885</v>
+      </c>
+      <c r="G15" s="40">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="14">
+        <v>895</v>
+      </c>
+      <c r="D16" s="14">
+        <v>888</v>
+      </c>
+      <c r="E16" s="14">
+        <v>887</v>
+      </c>
+      <c r="F16" s="14">
+        <v>885</v>
+      </c>
+      <c r="G16" s="15">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="40">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="15">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="13">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="13">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="13">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="13">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="40">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="14">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="14">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="14">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="14">
+        <v>20000</v>
+      </c>
+      <c r="F4" s="15">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1810,7 +3024,882 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15">
+        <v>50000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
+      <c r="I4" s="40">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13">
+        <v>2</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="40">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13">
+        <v>3</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="40"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="15">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="40">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="40">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="40">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="40">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31"/>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1827,8 +3916,10 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1845,8 +3936,10 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1863,8 +3956,10 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1881,6 +3976,48 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1890,308 +4027,307 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB6341-94DE-401B-89F3-66EA9EB6DBB9}">
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.28515625" style="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABFF4F0-1521-4984-985F-ECB7FE3DE71E}">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="14">
-        <v>31500</v>
-      </c>
-      <c r="C3" s="14">
-        <v>35000</v>
-      </c>
-      <c r="D3" s="14">
-        <v>35000</v>
-      </c>
-      <c r="E3" s="14">
-        <v>28000</v>
-      </c>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2201,109 +4337,528 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
extending get_data to read parameters with more than 2 indices
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -5,21 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1318ACA-6966-4CB6-AD73-ED7F1AAAFEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610F9474-B478-4D85-B782-CAF127E41A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="10" activeTab="10" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
     <sheet name="ProductionPads" sheetId="1" r:id="rId2"/>
-    <sheet name="CompletionsPads" sheetId="3" r:id="rId3"/>
-    <sheet name="SWDSites" sheetId="4" r:id="rId4"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId5"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId6"/>
-    <sheet name="FlowbackRates" sheetId="12" r:id="rId7"/>
+    <sheet name="ProductionTanks" sheetId="34" r:id="rId3"/>
+    <sheet name="CompletionsPads" sheetId="3" r:id="rId4"/>
+    <sheet name="SWDSites" sheetId="4" r:id="rId5"/>
+    <sheet name="FreshwaterSources" sheetId="35" r:id="rId6"/>
+    <sheet name="StorageSites" sheetId="36" r:id="rId7"/>
+    <sheet name="TreatmentSites" sheetId="37" r:id="rId8"/>
+    <sheet name="ReuseOptions" sheetId="38" r:id="rId9"/>
+    <sheet name="NetworkNodes" sheetId="39" r:id="rId10"/>
+    <sheet name="FCA" sheetId="41" r:id="rId11"/>
+    <sheet name="DriveTimes" sheetId="7" r:id="rId12"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId13"/>
+    <sheet name="ProductionRates" sheetId="40" r:id="rId14"/>
+    <sheet name="FlowbackRates" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -220,6 +228,78 @@
   </si>
   <si>
     <t>Table of Flowback Rates for Completion Pads over Weeks [bbl/day]</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>List of all Production Tank Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Freshwater Source Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Storage Site Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Treatment Site Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Reuse Option Identifiers [-]</t>
+  </si>
+  <si>
+    <t>List of all Network Node Identifiers [-]</t>
+  </si>
+  <si>
+    <t>Table of Production Rate Forecasts by Tanks and Pads [bbl/day]</t>
+  </si>
+  <si>
+    <t>Freshwater Sources to Completions Pads Arcs [-]</t>
   </si>
 </sst>
 </file>
@@ -306,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -470,12 +550,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,6 +667,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -894,15 +1066,15 @@
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.26171875" customWidth="1"/>
-    <col min="10" max="10" width="4.41796875" customWidth="1"/>
-    <col min="11" max="11" width="9.41796875" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -914,7 +1086,7 @@
       <c r="J2" s="19"/>
       <c r="K2" s="20"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="21"/>
       <c r="C3" s="22" t="s">
         <v>10</v>
@@ -928,7 +1100,7 @@
       <c r="J3" s="23"/>
       <c r="K3" s="24"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="21"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -940,7 +1112,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
       <c r="C5" s="23" t="s">
         <v>16</v>
@@ -954,7 +1126,7 @@
       <c r="J5" s="23"/>
       <c r="K5" s="24"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="21"/>
       <c r="C6" s="23" t="s">
         <v>14</v>
@@ -968,7 +1140,7 @@
       <c r="J6" s="23"/>
       <c r="K6" s="24"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="23" t="s">
         <v>11</v>
@@ -982,7 +1154,7 @@
       <c r="J7" s="23"/>
       <c r="K7" s="24"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
       <c r="C8" s="23" t="s">
         <v>12</v>
@@ -996,7 +1168,7 @@
       <c r="J8" s="23"/>
       <c r="K8" s="24"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="23" t="s">
         <v>13</v>
@@ -1010,7 +1182,7 @@
       <c r="J9" s="23"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="23" t="s">
         <v>52</v>
@@ -1024,7 +1196,7 @@
       <c r="J10" s="23"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -1036,7 +1208,7 @@
       <c r="J11" s="23"/>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
       <c r="C12" s="23" t="s">
         <v>17</v>
@@ -1050,7 +1222,7 @@
       <c r="J12" s="23"/>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="23" t="s">
         <v>15</v>
@@ -1064,7 +1236,7 @@
       <c r="J13" s="23"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -1076,7 +1248,7 @@
       <c r="J14" s="23"/>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="23" t="s">
         <v>18</v>
@@ -1090,7 +1262,7 @@
       <c r="J15" s="23"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="23" t="s">
         <v>19</v>
@@ -1104,7 +1276,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="23" t="s">
         <v>20</v>
@@ -1118,7 +1290,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="23" t="s">
         <v>21</v>
@@ -1132,7 +1304,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -1144,7 +1316,7 @@
       <c r="J19" s="23"/>
       <c r="K19" s="24"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -1156,7 +1328,7 @@
       <c r="J20" s="23"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="25" t="s">
         <v>22</v>
@@ -1172,7 +1344,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -1184,7 +1356,7 @@
       <c r="J22" s="23"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="26" t="s">
         <v>24</v>
@@ -1200,7 +1372,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="26" t="s">
         <v>25</v>
@@ -1216,7 +1388,7 @@
       <c r="J24" s="23"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="26" t="s">
         <v>26</v>
@@ -1232,7 +1404,7 @@
       <c r="J25" s="23"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="26" t="s">
         <v>30</v>
@@ -1248,7 +1420,7 @@
       <c r="J26" s="23"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="26" t="s">
         <v>32</v>
@@ -1264,7 +1436,7 @@
       <c r="J27" s="23"/>
       <c r="K27" s="24"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
       <c r="C28" s="26" t="s">
         <v>34</v>
@@ -1280,7 +1452,7 @@
       <c r="J28" s="23"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="21"/>
       <c r="C29" s="26" t="s">
         <v>35</v>
@@ -1296,7 +1468,7 @@
       <c r="J29" s="23"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="21"/>
       <c r="C30" s="26" t="s">
         <v>38</v>
@@ -1312,7 +1484,7 @@
       <c r="J30" s="23"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="21"/>
       <c r="C31" s="26" t="s">
         <v>40</v>
@@ -1331,7 +1503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="21"/>
       <c r="C32" s="26" t="s">
         <v>43</v>
@@ -1347,7 +1519,7 @@
       <c r="J32" s="23"/>
       <c r="K32" s="24"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="21"/>
       <c r="C33" s="26" t="s">
         <v>42</v>
@@ -1363,7 +1535,7 @@
       <c r="J33" s="23"/>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="21"/>
       <c r="C34" s="26" t="s">
         <v>46</v>
@@ -1379,7 +1551,7 @@
       <c r="J34" s="23"/>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="21"/>
       <c r="C35" s="26" t="s">
         <v>48</v>
@@ -1395,7 +1567,7 @@
       <c r="J35" s="23"/>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="21"/>
       <c r="C36" s="26" t="s">
         <v>49</v>
@@ -1411,7 +1583,7 @@
       <c r="J36" s="23"/>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -1445,175 +1617,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
-  <dimension ref="A1:R6"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.26171875" style="1"/>
-    <col min="3" max="3" width="3.578125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.26171875" style="1"/>
-    <col min="13" max="13" width="11.26171875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83984375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.578125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1633,7 +1667,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1653,7 +1687,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1673,7 +1707,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1693,7 +1727,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1713,7 +1747,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1733,7 +1767,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1754,44 +1788,937 @@
       <c r="T9" s="2"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="14">
+        <v>31500</v>
+      </c>
+      <c r="C3" s="14">
+        <v>35000</v>
+      </c>
+      <c r="D3" s="14">
+        <v>35000</v>
+      </c>
+      <c r="E3" s="14">
+        <v>28000</v>
+      </c>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB6341-94DE-401B-89F3-66EA9EB6DBB9}">
-  <dimension ref="A1:R7"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="4.41796875" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.26171875" style="1"/>
-    <col min="15" max="15" width="12.15625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="2" width="9.28515625" style="12"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1058</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1029</v>
+      </c>
+      <c r="E3" s="13">
+        <v>999</v>
+      </c>
+      <c r="F3" s="13">
+        <v>998</v>
+      </c>
+      <c r="G3" s="40">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1058</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1029</v>
+      </c>
+      <c r="E4" s="13">
+        <v>999</v>
+      </c>
+      <c r="F4" s="13">
+        <v>998</v>
+      </c>
+      <c r="G4" s="40">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="13">
+        <v>466</v>
+      </c>
+      <c r="D5" s="13">
+        <v>460</v>
+      </c>
+      <c r="E5" s="13">
+        <v>458</v>
+      </c>
+      <c r="F5" s="13">
+        <v>457</v>
+      </c>
+      <c r="G5" s="40">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="13">
+        <v>466</v>
+      </c>
+      <c r="D6" s="13">
+        <v>460</v>
+      </c>
+      <c r="E6" s="13">
+        <v>458</v>
+      </c>
+      <c r="F6" s="13">
+        <v>457</v>
+      </c>
+      <c r="G6" s="40">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="13">
+        <v>466</v>
+      </c>
+      <c r="D7" s="13">
+        <v>460</v>
+      </c>
+      <c r="E7" s="13">
+        <v>458</v>
+      </c>
+      <c r="F7" s="13">
+        <v>457</v>
+      </c>
+      <c r="G7" s="40">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="13">
+        <v>200</v>
+      </c>
+      <c r="D8" s="13">
+        <v>199</v>
+      </c>
+      <c r="E8" s="13">
+        <v>198</v>
+      </c>
+      <c r="F8" s="13">
+        <v>196</v>
+      </c>
+      <c r="G8" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="13">
+        <v>200</v>
+      </c>
+      <c r="D9" s="13">
+        <v>199</v>
+      </c>
+      <c r="E9" s="13">
+        <v>198</v>
+      </c>
+      <c r="F9" s="13">
+        <v>196</v>
+      </c>
+      <c r="G9" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="13">
+        <v>200</v>
+      </c>
+      <c r="D10" s="13">
+        <v>199</v>
+      </c>
+      <c r="E10" s="13">
+        <v>198</v>
+      </c>
+      <c r="F10" s="13">
+        <v>196</v>
+      </c>
+      <c r="G10" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="13">
+        <v>200</v>
+      </c>
+      <c r="D11" s="13">
+        <v>199</v>
+      </c>
+      <c r="E11" s="13">
+        <v>198</v>
+      </c>
+      <c r="F11" s="13">
+        <v>196</v>
+      </c>
+      <c r="G11" s="40">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="13">
+        <v>331</v>
+      </c>
+      <c r="D12" s="13">
+        <v>330</v>
+      </c>
+      <c r="E12" s="13">
+        <v>330</v>
+      </c>
+      <c r="F12" s="13">
+        <v>329</v>
+      </c>
+      <c r="G12" s="40">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="13">
+        <v>331</v>
+      </c>
+      <c r="D13" s="13">
+        <v>330</v>
+      </c>
+      <c r="E13" s="13">
+        <v>330</v>
+      </c>
+      <c r="F13" s="13">
+        <v>329</v>
+      </c>
+      <c r="G13" s="40">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="13">
+        <v>331</v>
+      </c>
+      <c r="D14" s="13">
+        <v>330</v>
+      </c>
+      <c r="E14" s="13">
+        <v>330</v>
+      </c>
+      <c r="F14" s="13">
+        <v>329</v>
+      </c>
+      <c r="G14" s="40">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="13">
+        <v>895</v>
+      </c>
+      <c r="D15" s="13">
+        <v>888</v>
+      </c>
+      <c r="E15" s="13">
+        <v>887</v>
+      </c>
+      <c r="F15" s="13">
+        <v>885</v>
+      </c>
+      <c r="G15" s="40">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="14">
+        <v>895</v>
+      </c>
+      <c r="D16" s="14">
+        <v>888</v>
+      </c>
+      <c r="E16" s="14">
+        <v>887</v>
+      </c>
+      <c r="F16" s="14">
+        <v>885</v>
+      </c>
+      <c r="G16" s="15">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1810,7 +2737,310 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1827,8 +3057,10 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1845,8 +3077,10 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1863,8 +3097,10 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1881,6 +3117,48 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1890,308 +3168,307 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB6341-94DE-401B-89F3-66EA9EB6DBB9}">
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.28515625" style="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABFF4F0-1521-4984-985F-ECB7FE3DE71E}">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="14">
-        <v>31500</v>
-      </c>
-      <c r="C3" s="14">
-        <v>35000</v>
-      </c>
-      <c r="D3" s="14">
-        <v>35000</v>
-      </c>
-      <c r="E3" s="14">
-        <v>28000</v>
-      </c>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2201,109 +3478,528 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
final removal of all hard-coded data from OPERATIONAL model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E0CD2F-F37E-4234-A637-FB7891D63C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E43D910-B1D5-420C-A5BA-559A9B31D350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="12" activeTab="21" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="22" activeTab="24" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -38,7 +38,6 @@
     <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId23"/>
     <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId24"/>
     <sheet name="FreshSourcingCost" sheetId="52" r:id="rId25"/>
-    <sheet name="FlowbackRates" sheetId="12" r:id="rId26"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="97">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -236,9 +235,6 @@
   </si>
   <si>
     <t>T5</t>
-  </si>
-  <si>
-    <t>Table of Flowback Rates for Completion Pads over Weeks [bbl/day]</t>
   </si>
   <si>
     <t>A01</t>
@@ -430,7 +426,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -508,19 +504,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -664,15 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,26 +677,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -725,13 +708,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1125,525 +1105,525 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
-      <c r="C6" s="23" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="24"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="23" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="24"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="23" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="24"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
-      <c r="C18" s="23" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="24"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="24"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="25" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="25" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="24"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="24"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="26" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="24"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="24"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="21"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
-      <c r="C25" s="26" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23" t="s">
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="24"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="21"/>
-      <c r="C26" s="26" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="24"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="21"/>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="24"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="21"/>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23" t="s">
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="24"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="21"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23" t="s">
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="24"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="21"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="24"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="21"/>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="18"/>
+      <c r="C31" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23" t="s">
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="24"/>
-      <c r="M31" s="30" t="s">
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="21"/>
+      <c r="M31" s="27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="21"/>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23" t="s">
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="24"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="21"/>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="18"/>
+      <c r="C33" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23" t="s">
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="24"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="21"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="21"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23" t="s">
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="24"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="21"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="21"/>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23" t="s">
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="24"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="21"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="21"/>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23" t="s">
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="24"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="21"/>
     </row>
     <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="29"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1690,14 +1670,14 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1709,9 +1689,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -1858,28 +1838,28 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1902,52 +1882,52 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1973,62 +1953,62 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="40"/>
-    </row>
-    <row r="4" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="C3" s="37"/>
+    </row>
+    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="40">
+      <c r="B5" s="38"/>
+      <c r="C5" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="40">
+      <c r="B6" s="38"/>
+      <c r="C6" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="15">
+      <c r="B7" s="39"/>
+      <c r="C7" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2053,20 +2033,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2091,174 +2071,174 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    </row>
+    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="40"/>
-    </row>
-    <row r="4" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="37"/>
+    </row>
+    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>1</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="40"/>
-    </row>
-    <row r="5" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="37"/>
+    </row>
+    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
         <v>1</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="10">
         <v>1</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="10">
         <v>1</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="40"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="37"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10">
         <v>1</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="10">
         <v>1</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="10">
         <v>1</v>
       </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="40"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="37"/>
     </row>
     <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11">
         <v>1</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2287,41 +2267,41 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="11">
         <v>31500</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>35000</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="11">
         <v>35000</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>28000</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
@@ -2336,7 +2316,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="16"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
@@ -2385,353 +2365,353 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" style="12"/>
+    <col min="1" max="2" width="9.28515625" style="9"/>
     <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="11" t="s">
+      <c r="A1" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1058</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1029</v>
+      </c>
+      <c r="E3" s="10">
+        <v>999</v>
+      </c>
+      <c r="F3" s="10">
+        <v>998</v>
+      </c>
+      <c r="G3" s="37">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C4" s="10">
         <v>1058</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D4" s="10">
         <v>1029</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E4" s="10">
         <v>999</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F4" s="10">
         <v>998</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G4" s="37">
         <v>996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="34" t="s">
+    <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="13">
-        <v>1058</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1029</v>
-      </c>
-      <c r="E4" s="13">
-        <v>999</v>
-      </c>
-      <c r="F4" s="13">
-        <v>998</v>
-      </c>
-      <c r="G4" s="40">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="C5" s="10">
+        <v>466</v>
+      </c>
+      <c r="D5" s="10">
+        <v>460</v>
+      </c>
+      <c r="E5" s="10">
+        <v>458</v>
+      </c>
+      <c r="F5" s="10">
+        <v>457</v>
+      </c>
+      <c r="G5" s="37">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B6" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C6" s="10">
         <v>466</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D6" s="10">
         <v>460</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E6" s="10">
         <v>458</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F6" s="10">
         <v>457</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G6" s="37">
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B7" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C7" s="10">
         <v>466</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D7" s="10">
         <v>460</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E7" s="10">
         <v>458</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F7" s="10">
         <v>457</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G7" s="37">
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="34" t="s">
+    <row r="8" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="13">
-        <v>466</v>
-      </c>
-      <c r="D7" s="13">
-        <v>460</v>
-      </c>
-      <c r="E7" s="13">
-        <v>458</v>
-      </c>
-      <c r="F7" s="13">
-        <v>457</v>
-      </c>
-      <c r="G7" s="40">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="C8" s="10">
+        <v>200</v>
+      </c>
+      <c r="D8" s="10">
+        <v>199</v>
+      </c>
+      <c r="E8" s="10">
+        <v>198</v>
+      </c>
+      <c r="F8" s="10">
+        <v>196</v>
+      </c>
+      <c r="G8" s="37">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C9" s="10">
         <v>200</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D9" s="10">
         <v>199</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E9" s="10">
         <v>198</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F9" s="10">
         <v>196</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G9" s="37">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B10" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C10" s="10">
         <v>200</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D10" s="10">
         <v>199</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E10" s="10">
         <v>198</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F10" s="10">
         <v>196</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G10" s="37">
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+    <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B11" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C11" s="10">
         <v>200</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D11" s="10">
         <v>199</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E11" s="10">
         <v>198</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F11" s="10">
         <v>196</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G11" s="37">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="34" t="s">
+    <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="13">
-        <v>200</v>
-      </c>
-      <c r="D11" s="13">
-        <v>199</v>
-      </c>
-      <c r="E11" s="13">
-        <v>198</v>
-      </c>
-      <c r="F11" s="13">
-        <v>196</v>
-      </c>
-      <c r="G11" s="40">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="C12" s="10">
+        <v>331</v>
+      </c>
+      <c r="D12" s="10">
+        <v>330</v>
+      </c>
+      <c r="E12" s="10">
+        <v>330</v>
+      </c>
+      <c r="F12" s="10">
+        <v>329</v>
+      </c>
+      <c r="G12" s="37">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B13" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C13" s="10">
         <v>331</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D13" s="10">
         <v>330</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E13" s="10">
         <v>330</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F13" s="10">
         <v>329</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G13" s="37">
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+    <row r="14" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B14" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C14" s="10">
         <v>331</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D14" s="10">
         <v>330</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E14" s="10">
         <v>330</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F14" s="10">
         <v>329</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G14" s="37">
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="34" t="s">
+    <row r="15" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="13">
-        <v>331</v>
-      </c>
-      <c r="D14" s="13">
-        <v>330</v>
-      </c>
-      <c r="E14" s="13">
-        <v>330</v>
-      </c>
-      <c r="F14" s="13">
-        <v>329</v>
-      </c>
-      <c r="G14" s="40">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="C15" s="10">
+        <v>895</v>
+      </c>
+      <c r="D15" s="10">
+        <v>888</v>
+      </c>
+      <c r="E15" s="10">
+        <v>887</v>
+      </c>
+      <c r="F15" s="10">
+        <v>885</v>
+      </c>
+      <c r="G15" s="37">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C16" s="11">
         <v>895</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D16" s="11">
         <v>888</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E16" s="11">
         <v>887</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F16" s="11">
         <v>885</v>
       </c>
-      <c r="G15" s="40">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="14">
-        <v>895</v>
-      </c>
-      <c r="D16" s="14">
-        <v>888</v>
-      </c>
-      <c r="E16" s="14">
-        <v>887</v>
-      </c>
-      <c r="F16" s="14">
-        <v>885</v>
-      </c>
-      <c r="G16" s="15">
+      <c r="G16" s="12">
         <v>883</v>
       </c>
     </row>
@@ -2748,7 +2728,7 @@
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="16"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
@@ -2801,26 +2781,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31"/>
-    </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="37">
         <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>10000</v>
       </c>
     </row>
@@ -2845,64 +2825,64 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="37">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="13">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="13">
-        <v>30000</v>
-      </c>
-      <c r="D3" s="13">
-        <v>30000</v>
-      </c>
-      <c r="E3" s="13">
-        <v>30000</v>
-      </c>
-      <c r="F3" s="40">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>20000</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>20000</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>20000</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>20000</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="12">
         <v>20000</v>
       </c>
     </row>
@@ -2919,7 +2899,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="16"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
@@ -2983,7 +2963,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2"/>
@@ -3004,7 +2984,7 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
@@ -3025,11 +3005,11 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3046,7 +3026,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2"/>
@@ -3059,15 +3039,15 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2"/>
@@ -3109,18 +3089,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>50000</v>
       </c>
     </row>
@@ -3149,157 +3129,157 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
         <v>1</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="10">
         <v>1.5</v>
       </c>
-      <c r="I3" s="40"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
         <v>1.5</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="10">
         <v>1</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="37">
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
         <v>2</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="40">
+      <c r="H5" s="10"/>
+      <c r="I5" s="37">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
         <v>2.5</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="40">
+      <c r="H6" s="10"/>
+      <c r="I6" s="37">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
         <v>3</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="40">
+      <c r="H7" s="10"/>
+      <c r="I7" s="37">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="40"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="40"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="37"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
@@ -3319,7 +3299,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
@@ -3361,7 +3341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3370,26 +3350,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31"/>
-    </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="37">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>8</v>
       </c>
     </row>
@@ -3414,18 +3394,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>1.2</v>
       </c>
     </row>
@@ -3450,58 +3430,58 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="37">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31"/>
-    </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="40">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="40">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="37">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="37">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="37">
         <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>92</v>
       </c>
     </row>
@@ -3515,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3526,139 +3506,30 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="31"/>
-    </row>
-    <row r="3" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="40">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
-  <dimension ref="A1:F19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3686,12 +3557,12 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>63</v>
+      <c r="A2" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3711,8 +3582,8 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>64</v>
+      <c r="A3" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3732,11 +3603,11 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>65</v>
+      <c r="A4" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3753,8 +3624,8 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>66</v>
+      <c r="A5" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -3766,16 +3637,16 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>67</v>
+      <c r="A6" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3795,48 +3666,48 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3873,7 +3744,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3889,9 +3760,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -4049,12 +3920,12 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="2"/>
@@ -4176,17 +4047,17 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4199,9 +4070,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -4357,14 +4228,14 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4376,9 +4247,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -4533,14 +4404,14 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4552,9 +4423,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -4709,14 +4580,14 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4728,9 +4599,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>

</xml_diff>

<commit_message>
completions storage for operational model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2762D9C9-077E-43F5-A282-2C8345EF2905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91548001-56B9-46C5-A180-0E3962EBB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="20" activeTab="26" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="17" activeTab="19" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -32,14 +32,15 @@
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId17"/>
     <sheet name="ProductionRates" sheetId="40" r:id="rId18"/>
     <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId19"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId20"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId21"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId22"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId23"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId24"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId25"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId26"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId27"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId20"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId21"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId22"/>
+    <sheet name="DriveTimes" sheetId="7" r:id="rId23"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId24"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId25"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId26"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId27"/>
+    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId28"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="100">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -348,6 +349,9 @@
   </si>
   <si>
     <t>Piping Operational Costs [$/bbl]</t>
+  </si>
+  <si>
+    <t>Table of Completions Pad Storage Capacity  [bbl]</t>
   </si>
 </sst>
 </file>
@@ -3002,6 +3006,42 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -3128,7 +3168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3164,7 +3204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -3421,7 +3461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3463,7 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3499,7 +3539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -3591,7 +3631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3635,11 +3675,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
initial attempt equalized tank modeling
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91548001-56B9-46C5-A180-0E3962EBB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D36D56-B655-482D-AE30-80F494B8BA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="17" activeTab="19" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="15" activeTab="18" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -31,28 +31,38 @@
     <sheet name="PAL" sheetId="45" r:id="rId16"/>
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId17"/>
     <sheet name="ProductionRates" sheetId="40" r:id="rId18"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId19"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId20"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId21"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId22"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId23"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId24"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId25"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId26"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId27"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId28"/>
+    <sheet name="PadRates" sheetId="56" r:id="rId19"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId20"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId21"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId22"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId23"/>
+    <sheet name="DriveTimes" sheetId="7" r:id="rId24"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId25"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId26"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId27"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId28"/>
+    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId29"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="101">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -352,6 +362,9 @@
   </si>
   <si>
     <t>Table of Completions Pad Storage Capacity  [bbl]</t>
+  </si>
+  <si>
+    <t>Table of Production Rate Forecasts by Pads [bbl/day]</t>
   </si>
 </sst>
 </file>
@@ -2825,42 +2838,186 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="9"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="37">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="12">
-        <v>10000</v>
-      </c>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2116</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2058</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1998</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1996</v>
+      </c>
+      <c r="F3" s="37">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1398</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1380</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1374</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1371</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10">
+        <v>800</v>
+      </c>
+      <c r="C5" s="10">
+        <v>796</v>
+      </c>
+      <c r="D5" s="10">
+        <v>792</v>
+      </c>
+      <c r="E5" s="10">
+        <v>784</v>
+      </c>
+      <c r="F5" s="37">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10">
+        <v>993</v>
+      </c>
+      <c r="C6" s="10">
+        <v>990</v>
+      </c>
+      <c r="D6" s="10">
+        <v>990</v>
+      </c>
+      <c r="E6" s="10">
+        <v>987</v>
+      </c>
+      <c r="F6" s="37">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1790</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1776</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1774</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1770</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3006,10 +3163,54 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="37">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3041,7 +3242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -3168,7 +3369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3204,7 +3405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -3461,7 +3662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3503,7 +3704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3539,7 +3740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -3631,7 +3832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3675,7 +3876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
example to use config dictionary
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MZamarripa\Documents\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B598AAE-7DC2-441B-A451-2E3131894280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667FF175-920A-4708-A75E-9476495B1103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="15" activeTab="18" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="3870" yWindow="150" windowWidth="28395" windowHeight="20595" firstSheet="12" activeTab="20" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <sheet name="ProductionRates" sheetId="40" r:id="rId17"/>
     <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId18"/>
     <sheet name="DriveTimes" sheetId="7" r:id="rId19"/>
-    <sheet name="FlowbackRates" sheetId="12" r:id="rId20"/>
+    <sheet name="PadRates" sheetId="47" r:id="rId20"/>
+    <sheet name="CompletionsPadStorage" sheetId="48" r:id="rId21"/>
+    <sheet name="FlowbackRates" sheetId="12" r:id="rId22"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="94">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -320,6 +322,12 @@
   </si>
   <si>
     <t>Table of Initial Disposal Capacity  [bbl/day]</t>
+  </si>
+  <si>
+    <t>Table of Production Rate Forecasts by Pads [bbl/week]</t>
+  </si>
+  <si>
+    <t>Table of Completoins Pad Storage Capacity  [bbl]</t>
   </si>
 </sst>
 </file>
@@ -640,7 +648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -720,6 +728,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2808,7 +2861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -3169,6 +3222,122 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC9779A-715A-4537-8C85-851D795D6791}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="46">
+        <v>14000</v>
+      </c>
+      <c r="C3" s="46">
+        <v>13800</v>
+      </c>
+      <c r="D3" s="46">
+        <v>13750</v>
+      </c>
+      <c r="E3" s="46">
+        <v>13700</v>
+      </c>
+      <c r="F3" s="53">
+        <v>13650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="47">
+        <v>8000</v>
+      </c>
+      <c r="C4" s="47">
+        <v>7950</v>
+      </c>
+      <c r="D4" s="47">
+        <v>7900</v>
+      </c>
+      <c r="E4" s="47">
+        <v>7850</v>
+      </c>
+      <c r="F4" s="48">
+        <v>7800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50069B37-E30D-4815-801D-ED977AA656AE}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="54"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="56"/>
+      <c r="B2" s="58"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="57">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AB1186-A1E7-4C17-BA8E-EB0106BA7D22}">
   <dimension ref="A1:F19"/>
   <sheetViews>

</xml_diff>

<commit_message>
equalized production tank formulation
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91548001-56B9-46C5-A180-0E3962EBB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D36D56-B655-482D-AE30-80F494B8BA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="17" activeTab="19" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="15" activeTab="18" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -31,28 +31,38 @@
     <sheet name="PAL" sheetId="45" r:id="rId16"/>
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId17"/>
     <sheet name="ProductionRates" sheetId="40" r:id="rId18"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId19"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId20"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId21"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId22"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId23"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId24"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId25"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId26"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId27"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId28"/>
+    <sheet name="PadRates" sheetId="56" r:id="rId19"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId20"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId21"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId22"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId23"/>
+    <sheet name="DriveTimes" sheetId="7" r:id="rId24"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId25"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId26"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId27"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId28"/>
+    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId29"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="101">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -352,6 +362,9 @@
   </si>
   <si>
     <t>Table of Completions Pad Storage Capacity  [bbl]</t>
+  </si>
+  <si>
+    <t>Table of Production Rate Forecasts by Pads [bbl/day]</t>
   </si>
 </sst>
 </file>
@@ -2825,42 +2838,186 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="9"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="37">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="12">
-        <v>10000</v>
-      </c>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2116</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2058</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1998</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1996</v>
+      </c>
+      <c r="F3" s="37">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1398</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1380</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1374</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1371</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10">
+        <v>800</v>
+      </c>
+      <c r="C5" s="10">
+        <v>796</v>
+      </c>
+      <c r="D5" s="10">
+        <v>792</v>
+      </c>
+      <c r="E5" s="10">
+        <v>784</v>
+      </c>
+      <c r="F5" s="37">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10">
+        <v>993</v>
+      </c>
+      <c r="C6" s="10">
+        <v>990</v>
+      </c>
+      <c r="D6" s="10">
+        <v>990</v>
+      </c>
+      <c r="E6" s="10">
+        <v>987</v>
+      </c>
+      <c r="F6" s="37">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1790</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1776</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1774</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1770</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3006,10 +3163,54 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="37">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3041,7 +3242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -3168,7 +3369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3204,7 +3405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -3461,7 +3662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3503,7 +3704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3539,7 +3740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -3631,7 +3832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3675,7 +3876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
improved flowback processing - operational
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drouvenm\PARETO\GitHub\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D36D56-B655-482D-AE30-80F494B8BA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9BACFE-A529-41F1-ADBD-7BF1A0559356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="300" windowWidth="37200" windowHeight="20700" firstSheet="15" activeTab="18" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="8" activeTab="20" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -26,22 +26,24 @@
     <sheet name="FCA" sheetId="41" r:id="rId11"/>
     <sheet name="PCT" sheetId="42" r:id="rId12"/>
     <sheet name="FCT" sheetId="53" r:id="rId13"/>
-    <sheet name="PKT" sheetId="43" r:id="rId14"/>
-    <sheet name="CKT" sheetId="44" r:id="rId15"/>
-    <sheet name="PAL" sheetId="45" r:id="rId16"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId17"/>
-    <sheet name="ProductionRates" sheetId="40" r:id="rId18"/>
-    <sheet name="PadRates" sheetId="56" r:id="rId19"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId20"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId21"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId22"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId23"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId24"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId25"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId26"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId27"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId28"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId29"/>
+    <sheet name="CCT" sheetId="57" r:id="rId14"/>
+    <sheet name="PKT" sheetId="43" r:id="rId15"/>
+    <sheet name="CKT" sheetId="44" r:id="rId16"/>
+    <sheet name="PAL" sheetId="45" r:id="rId17"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId18"/>
+    <sheet name="ProductionRates" sheetId="40" r:id="rId19"/>
+    <sheet name="PadRates" sheetId="56" r:id="rId20"/>
+    <sheet name="FlowbackRates" sheetId="58" r:id="rId21"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId22"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId23"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId24"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId25"/>
+    <sheet name="DriveTimes" sheetId="7" r:id="rId26"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId27"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId28"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId29"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId30"/>
+    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="102">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -365,6 +367,9 @@
   </si>
   <si>
     <t>Table of Production Rate Forecasts by Pads [bbl/day]</t>
+  </si>
+  <si>
+    <t>Table of Flowback Rate Forecasts by Pads [bbl/day]</t>
   </si>
 </sst>
 </file>
@@ -1898,7 +1903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1968,7 +1975,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2010,11 +2017,49 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16082D3-6CFF-4538-9513-170B327E5C50}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2127,7 +2172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABD83BE-FC18-4B07-A835-FE113535C483}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -2320,7 +2365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -2426,7 +2471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -2837,200 +2882,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
-  <dimension ref="A1:F18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.28515625" style="9"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10">
-        <v>2116</v>
-      </c>
-      <c r="C3" s="10">
-        <v>2058</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1998</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1996</v>
-      </c>
-      <c r="F3" s="37">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1398</v>
-      </c>
-      <c r="C4" s="10">
-        <v>1380</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1374</v>
-      </c>
-      <c r="E4" s="10">
-        <v>1371</v>
-      </c>
-      <c r="F4" s="37">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="10">
-        <v>800</v>
-      </c>
-      <c r="C5" s="10">
-        <v>796</v>
-      </c>
-      <c r="D5" s="10">
-        <v>792</v>
-      </c>
-      <c r="E5" s="10">
-        <v>784</v>
-      </c>
-      <c r="F5" s="37">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10">
-        <v>993</v>
-      </c>
-      <c r="C6" s="10">
-        <v>990</v>
-      </c>
-      <c r="D6" s="10">
-        <v>990</v>
-      </c>
-      <c r="E6" s="10">
-        <v>987</v>
-      </c>
-      <c r="F6" s="37">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="11">
-        <v>1790</v>
-      </c>
-      <c r="C7" s="11">
-        <v>1776</v>
-      </c>
-      <c r="D7" s="11">
-        <v>1774</v>
-      </c>
-      <c r="E7" s="11">
-        <v>1770</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3163,6 +3020,302 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" style="9"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2116</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2058</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1998</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1996</v>
+      </c>
+      <c r="F3" s="37">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1398</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1380</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1374</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1371</v>
+      </c>
+      <c r="F4" s="37">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10">
+        <v>800</v>
+      </c>
+      <c r="C5" s="10">
+        <v>796</v>
+      </c>
+      <c r="D5" s="10">
+        <v>792</v>
+      </c>
+      <c r="E5" s="10">
+        <v>784</v>
+      </c>
+      <c r="F5" s="37">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10">
+        <v>993</v>
+      </c>
+      <c r="C6" s="10">
+        <v>990</v>
+      </c>
+      <c r="D6" s="10">
+        <v>990</v>
+      </c>
+      <c r="E6" s="10">
+        <v>987</v>
+      </c>
+      <c r="F6" s="37">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1790</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1776</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1774</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1770</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" style="9"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="11">
+        <v>500</v>
+      </c>
+      <c r="C3" s="11">
+        <v>500</v>
+      </c>
+      <c r="D3" s="11">
+        <v>500</v>
+      </c>
+      <c r="E3" s="11">
+        <v>500</v>
+      </c>
+      <c r="F3" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3206,7 +3359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3242,7 +3395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -3369,12 +3522,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3405,17 +3558,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="6" width="9.28515625" style="1"/>
+    <col min="7" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3546,8 +3701,12 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="10">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H8" s="10">
+        <v>2</v>
+      </c>
       <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3662,7 +3821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3704,7 +3863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3740,7 +3899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -3824,96 +3983,6 @@
       </c>
       <c r="B10" s="12">
         <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0.85</v>
       </c>
     </row>
   </sheetData>
@@ -4099,6 +4168,96 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding pad storage cost
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calderoa\Documents\KeyLogic\PARETO\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54325818ffabb65a/Documents/KeyLogic/PARETO/project-pareto/pareto/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775EE0FE-EAB7-4B1B-B842-5C99B4DAD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{775EE0FE-EAB7-4B1B-B842-5C99B4DAD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A18D749-C590-4598-959C-28F5A4271A03}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="770" firstSheet="26" activeTab="31" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="30" activeTab="34" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -47,15 +47,25 @@
     <sheet name="DriveTimes" sheetId="7" r:id="rId32"/>
     <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId33"/>
     <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId34"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId35"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId36"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId37"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId38"/>
+    <sheet name="PadStorageCost" sheetId="67" r:id="rId35"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId36"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId37"/>
+    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId38"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId39"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -226,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="119">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -580,6 +590,9 @@
   </si>
   <si>
     <t>NODES</t>
+  </si>
+  <si>
+    <t>Table of Completions Pad Storage Capacity over Time [bbl]</t>
   </si>
 </sst>
 </file>
@@ -692,7 +705,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -908,12 +921,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -994,6 +1020,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1358,21 +1393,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E5E074-61D5-4D82-B0DB-255C2595EBED}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:M37"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.26171875" customWidth="1"/>
-    <col min="10" max="10" width="4.41796875" customWidth="1"/>
-    <col min="11" max="11" width="9.41796875" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -1384,7 +1420,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="19" t="s">
         <v>10</v>
@@ -1398,7 +1434,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="21"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="18"/>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -1410,7 +1446,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="21"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="18"/>
       <c r="C5" s="20" t="s">
         <v>16</v>
@@ -1424,7 +1460,7 @@
       <c r="J5" s="20"/>
       <c r="K5" s="21"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="18"/>
       <c r="C6" s="20" t="s">
         <v>14</v>
@@ -1438,7 +1474,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="21"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="18"/>
       <c r="C7" s="20" t="s">
         <v>11</v>
@@ -1452,7 +1488,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="18"/>
       <c r="C8" s="20" t="s">
         <v>12</v>
@@ -1466,7 +1502,7 @@
       <c r="J8" s="20"/>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="18"/>
       <c r="C9" s="20" t="s">
         <v>13</v>
@@ -1480,7 +1516,7 @@
       <c r="J9" s="20"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="18"/>
       <c r="C10" s="20" t="s">
         <v>52</v>
@@ -1494,7 +1530,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="18"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -1506,7 +1542,7 @@
       <c r="J11" s="20"/>
       <c r="K11" s="21"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="18"/>
       <c r="C12" s="20" t="s">
         <v>17</v>
@@ -1520,7 +1556,7 @@
       <c r="J12" s="20"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
       <c r="C13" s="20" t="s">
         <v>15</v>
@@ -1534,7 +1570,7 @@
       <c r="J13" s="20"/>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="18"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -1546,7 +1582,7 @@
       <c r="J14" s="20"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="C15" s="20" t="s">
         <v>18</v>
@@ -1560,7 +1596,7 @@
       <c r="J15" s="20"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
         <v>19</v>
@@ -1574,7 +1610,7 @@
       <c r="J16" s="20"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="18"/>
       <c r="C17" s="20" t="s">
         <v>20</v>
@@ -1588,7 +1624,7 @@
       <c r="J17" s="20"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="18"/>
       <c r="C18" s="20" t="s">
         <v>21</v>
@@ -1602,7 +1638,7 @@
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="18"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -1614,7 +1650,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="18"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
@@ -1626,7 +1662,7 @@
       <c r="J20" s="20"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
         <v>22</v>
@@ -1642,7 +1678,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="18"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -1654,7 +1690,7 @@
       <c r="J22" s="20"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="18"/>
       <c r="C23" s="23" t="s">
         <v>24</v>
@@ -1670,7 +1706,7 @@
       <c r="J23" s="20"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="18"/>
       <c r="C24" s="23" t="s">
         <v>25</v>
@@ -1686,7 +1722,7 @@
       <c r="J24" s="20"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="18"/>
       <c r="C25" s="23" t="s">
         <v>26</v>
@@ -1702,7 +1738,7 @@
       <c r="J25" s="20"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="18"/>
       <c r="C26" s="23" t="s">
         <v>30</v>
@@ -1718,7 +1754,7 @@
       <c r="J26" s="20"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="18"/>
       <c r="C27" s="23" t="s">
         <v>32</v>
@@ -1734,7 +1770,7 @@
       <c r="J27" s="20"/>
       <c r="K27" s="21"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="18"/>
       <c r="C28" s="23" t="s">
         <v>34</v>
@@ -1750,7 +1786,7 @@
       <c r="J28" s="20"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="18"/>
       <c r="C29" s="23" t="s">
         <v>35</v>
@@ -1766,7 +1802,7 @@
       <c r="J29" s="20"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="18"/>
       <c r="C30" s="23" t="s">
         <v>38</v>
@@ -1782,7 +1818,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="18"/>
       <c r="C31" s="23" t="s">
         <v>40</v>
@@ -1801,7 +1837,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="18"/>
       <c r="C32" s="23" t="s">
         <v>43</v>
@@ -1817,7 +1853,7 @@
       <c r="J32" s="20"/>
       <c r="K32" s="21"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="18"/>
       <c r="C33" s="23" t="s">
         <v>42</v>
@@ -1833,7 +1869,7 @@
       <c r="J33" s="20"/>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="18"/>
       <c r="C34" s="23" t="s">
         <v>46</v>
@@ -1849,7 +1885,7 @@
       <c r="J34" s="20"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="18"/>
       <c r="C35" s="23" t="s">
         <v>48</v>
@@ -1865,7 +1901,7 @@
       <c r="J35" s="20"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="18"/>
       <c r="C36" s="23" t="s">
         <v>49</v>
@@ -1881,7 +1917,7 @@
       <c r="J36" s="20"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
@@ -1917,36 +1953,37 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABFF4F0-1521-4984-985F-ECB7FE3DE71E}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>77</v>
       </c>
@@ -1969,7 +2006,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1989,7 +2026,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2009,7 +2046,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2029,7 +2066,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2049,7 +2086,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2069,7 +2106,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2098,34 +2135,35 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2146,7 +2184,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2166,7 +2204,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2186,7 +2224,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2206,7 +2244,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2226,7 +2264,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2246,7 +2284,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2274,34 +2312,35 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2322,7 +2361,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2342,7 +2381,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2362,7 +2401,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2382,7 +2421,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2402,7 +2441,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2422,7 +2461,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2450,15 +2489,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC3797B-8D14-4FB6-B72A-3C0C4341EC79}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -2470,15 +2510,16 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1A6821-D55E-4269-AC7B-EA9C0F0EC2AD}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -2490,34 +2531,35 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2538,7 +2580,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2558,7 +2600,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2578,7 +2620,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2598,7 +2640,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2618,7 +2660,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2638,7 +2680,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2666,34 +2708,35 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2714,7 +2757,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2734,7 +2777,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2754,7 +2797,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2774,7 +2817,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2794,7 +2837,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2814,7 +2857,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2842,19 +2885,20 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -2862,7 +2906,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -2871,7 +2915,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>76</v>
       </c>
@@ -2885,7 +2929,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>77</v>
       </c>
@@ -2897,7 +2941,7 @@
         <v>2.083333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>106</v>
       </c>
@@ -2908,12 +2952,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="41" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="41">
         <v>1</v>
       </c>
@@ -2927,19 +2971,20 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.05078125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -2947,7 +2992,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>109</v>
       </c>
@@ -2955,7 +3000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
@@ -2963,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -2971,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -2979,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
@@ -2987,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
@@ -2995,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="40" t="s">
         <v>106</v>
       </c>
@@ -3009,23 +3054,24 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -3033,7 +3079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>76</v>
       </c>
@@ -3041,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>77</v>
       </c>
@@ -3059,23 +3105,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="9.26171875" style="1"/>
-    <col min="10" max="10" width="11.26171875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.68359375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83984375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="9" width="9.21875" style="1"/>
+    <col min="10" max="10" width="11.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3083,7 +3130,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -3101,7 +3148,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -3119,7 +3166,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -3140,7 +3187,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -3158,7 +3205,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -3176,7 +3223,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="s">
         <v>106</v>
       </c>
@@ -3193,23 +3240,24 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16082D3-6CFF-4538-9513-170B327E5C50}">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -3217,7 +3265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
@@ -3233,24 +3281,25 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>109</v>
       </c>
@@ -3261,7 +3310,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
@@ -3270,7 +3319,7 @@
       </c>
       <c r="C3" s="37"/>
     </row>
-    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -3281,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -3290,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
@@ -3299,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
@@ -3316,23 +3365,24 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -3340,7 +3390,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
@@ -3356,24 +3406,25 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABD83BE-FC18-4B07-A835-FE113535C483}">
+  <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.62890625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>109</v>
       </c>
@@ -3420,7 +3471,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>3</v>
       </c>
@@ -3443,7 +3494,7 @@
       <c r="N3" s="10"/>
       <c r="O3" s="37"/>
     </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -3468,7 +3519,7 @@
       <c r="N4" s="10"/>
       <c r="O4" s="37"/>
     </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -3495,7 +3546,7 @@
       <c r="N5" s="10"/>
       <c r="O5" s="37"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
@@ -3520,7 +3571,7 @@
       <c r="N6" s="10"/>
       <c r="O6" s="37"/>
     </row>
-    <row r="7" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
@@ -3552,20 +3603,21 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
+  <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="9.26171875" style="1"/>
-    <col min="8" max="8" width="22.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="7" width="9.21875" style="1"/>
+    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -3573,7 +3625,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -3593,7 +3645,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -3613,47 +3665,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -3667,20 +3719,21 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
+  <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.15625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="22.9453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="18.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>84</v>
       </c>
@@ -3688,7 +3741,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>109</v>
       </c>
@@ -3711,7 +3764,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>3</v>
       </c>
@@ -3734,7 +3787,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -3757,7 +3810,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>4</v>
       </c>
@@ -3780,7 +3833,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>4</v>
       </c>
@@ -3803,7 +3856,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
@@ -3826,7 +3879,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>5</v>
       </c>
@@ -3849,7 +3902,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>5</v>
       </c>
@@ -3872,7 +3925,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>5</v>
       </c>
@@ -3895,7 +3948,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>5</v>
       </c>
@@ -3918,7 +3971,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>6</v>
       </c>
@@ -3941,7 +3994,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>6</v>
       </c>
@@ -3964,7 +4017,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>6</v>
       </c>
@@ -3987,7 +4040,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
@@ -4010,7 +4063,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34" t="s">
         <v>7</v>
       </c>
@@ -4033,47 +4086,47 @@
         <v>883</v>
       </c>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -4086,24 +4139,25 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
+  <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1015625" style="9" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="17.109375" style="9" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>109</v>
       </c>
@@ -4123,7 +4177,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>3</v>
       </c>
@@ -4143,7 +4197,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -4163,7 +4217,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -4183,7 +4237,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
@@ -4203,7 +4257,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
@@ -4223,47 +4277,47 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -4276,24 +4330,25 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
+  <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.26171875" style="9"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="9.21875" style="9"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -4313,7 +4368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
@@ -4333,47 +4388,47 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -4386,18 +4441,19 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
+  <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -4408,7 +4464,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>113</v>
       </c>
@@ -4419,7 +4475,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>54</v>
       </c>
@@ -4427,7 +4483,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>55</v>
       </c>
@@ -4438,7 +4494,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
         <v>106</v>
       </c>
@@ -4457,36 +4513,61 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
-  <dimension ref="A1:B3"/>
+  <sheetPr codeName="Sheet29"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1015625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="43">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="43">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="43">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="43">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="44">
         <v>10000</v>
       </c>
     </row>
@@ -4498,30 +4579,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.26171875" style="1"/>
-    <col min="3" max="3" width="3.578125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.26171875" style="1"/>
-    <col min="13" max="13" width="11.26171875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83984375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.578125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="2" width="9.21875" style="1"/>
+    <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.21875" style="1"/>
+    <col min="13" max="13" width="11.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -4542,7 +4624,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
@@ -4563,7 +4645,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>64</v>
       </c>
@@ -4584,7 +4666,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>65</v>
       </c>
@@ -4605,7 +4687,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>66</v>
       </c>
@@ -4626,47 +4708,47 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>75</v>
       </c>
@@ -4680,24 +4762,25 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
+  <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.9453125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
@@ -4717,7 +4800,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>76</v>
       </c>
@@ -4737,7 +4820,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>77</v>
       </c>
@@ -4757,47 +4840,47 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -4810,24 +4893,25 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
+  <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7890625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -4835,7 +4919,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
@@ -4851,26 +4935,27 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <sheetPr codeName="Sheet32"/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7890625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.26171875" style="1"/>
-    <col min="7" max="8" width="13.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.21875" style="1"/>
+    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>117</v>
       </c>
@@ -4899,7 +4984,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4916,7 +5001,7 @@
       </c>
       <c r="I3" s="37"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -4935,7 +5020,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -4952,7 +5037,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4969,7 +5054,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -4986,7 +5071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -5003,7 +5088,7 @@
       </c>
       <c r="I8" s="37"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>76</v>
       </c>
@@ -5018,7 +5103,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="37"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -5033,7 +5118,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>54</v>
       </c>
@@ -5046,7 +5131,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="37"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>55</v>
       </c>
@@ -5059,52 +5144,52 @@
       <c r="H12" s="11"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -5117,23 +5202,24 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
+  <sheetPr codeName="Sheet33"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>113</v>
       </c>
@@ -5141,7 +5227,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>54</v>
       </c>
@@ -5149,7 +5235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>55</v>
       </c>
@@ -5165,24 +5251,25 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
+  <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.89453125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -5190,7 +5277,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
@@ -5205,93 +5292,63 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5A0C0B-D826-45D7-BBE7-9638BF5673C5}">
+  <sheetPr codeName="Sheet39"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="37">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="37">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="37">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="37">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="37">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="37">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="37">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="12">
-        <v>92</v>
+      <c r="B3" s="43">
+        <v>250</v>
+      </c>
+      <c r="C3" s="43">
+        <v>250</v>
+      </c>
+      <c r="D3" s="43">
+        <v>250</v>
+      </c>
+      <c r="E3" s="43">
+        <v>250</v>
+      </c>
+      <c r="F3" s="44">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -5301,46 +5358,94 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
+  <sheetPr codeName="Sheet35"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5234375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="37">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="34" t="s">
+      <c r="B4" s="37">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="12">
-        <v>0.5</v>
+      <c r="B5" s="37">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="37">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="37">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="37">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="37">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="12">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -5350,45 +5455,47 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <sheetPr codeName="Sheet36"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="37">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="12">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -5398,14 +5505,64 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
+  <sheetPr codeName="Sheet37"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
+  <sheetPr codeName="Sheet38"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5413,15 +5570,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -5433,15 +5591,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59865970-D83F-46CB-8781-62CE35DBF4B5}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -5453,15 +5612,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517D4D1F-C9B2-48B7-BC2C-B9CAACD1B518}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -5473,13 +5633,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163385F3-A1AA-43A4-BCBF-5D7593716FB8}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5487,36 +5648,37 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="3.578125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.26171875" style="1"/>
-    <col min="14" max="14" width="12.68359375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.26171875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.41796875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -5536,7 +5698,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5556,7 +5718,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5576,7 +5738,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5596,7 +5758,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5616,7 +5778,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5636,7 +5798,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -5665,34 +5827,35 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB6341-94DE-401B-89F3-66EA9EB6DBB9}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26171875" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.26171875" style="1"/>
-    <col min="4" max="4" width="4.41796875" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.26171875" style="1"/>
-    <col min="15" max="15" width="12.15625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.26171875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.26171875" style="1"/>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.21875" style="1"/>
+    <col min="15" max="15" width="12.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -5713,7 +5876,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5731,7 +5894,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5749,7 +5912,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5767,7 +5930,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
add operational input tabs from main
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\GIT\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C445A22F-7A20-4D2E-BF41-5AC434AAB121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B7C44C-920B-493F-BF98-ED67F7278850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="770" firstSheet="13" activeTab="17" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="15" activeTab="17" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -53,6 +53,7 @@
     <sheet name="FreshSourcingCost" sheetId="52" r:id="rId38"/>
     <sheet name="PipingOperationalCost" sheetId="54" r:id="rId39"/>
     <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId40"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId41"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -237,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -609,6 +610,9 @@
   </si>
   <si>
     <t>VALUE</t>
+  </si>
+  <si>
+    <t>Table of Completions Pad Storage Capacity over Time [bbl]</t>
   </si>
 </sst>
 </file>
@@ -721,7 +725,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -937,12 +941,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1024,6 +1041,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3010,7 +3036,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3774,7 +3800,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4858,10 +4884,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4870,24 +4896,48 @@
     <col min="2" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="45">
         <v>10000</v>
       </c>
     </row>
@@ -5647,6 +5697,71 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="44">
+        <v>250</v>
+      </c>
+      <c r="C3" s="44">
+        <v>250</v>
+      </c>
+      <c r="D3" s="44">
+        <v>250</v>
+      </c>
+      <c r="E3" s="44">
+        <v>250</v>
+      </c>
+      <c r="F3" s="45">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add water quality calculation
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B7C44C-920B-493F-BF98-ED67F7278850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648661D6-5180-4413-8E0D-10D51FA44257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="15" activeTab="17" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="37" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -54,6 +54,7 @@
     <sheet name="PipingOperationalCost" sheetId="54" r:id="rId39"/>
     <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId40"/>
     <sheet name="PadStorageCost" sheetId="70" r:id="rId41"/>
+    <sheet name="WaterQuality" sheetId="71" r:id="rId42"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -238,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="128">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -613,13 +614,25 @@
   </si>
   <si>
     <t>Table of Completions Pad Storage Capacity over Time [bbl]</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Water Quality at Production Pads (mg/L)</t>
+  </si>
+  <si>
+    <t>Pads and Storage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +710,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -955,11 +975,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1052,8 +1073,18 @@
     <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3035,7 +3066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19482E4D-5604-4B83-9F7A-0225AC5DE7E0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -3800,7 +3831,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5758,6 +5789,123 @@
       <c r="F3" s="45">
         <v>250</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FA9205-AA30-4BB4-8EBD-7F4667959AD4}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="46">
+        <v>142277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="46">
+        <v>140998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="46">
+        <v>172490.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="46">
+        <v>257547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="46">
+        <v>241833.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="48">
+        <v>188503.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+      <c r="B9" s="46"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="30"/>
+      <c r="B10" s="46"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="46"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="46"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+      <c r="B13" s="46"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="46"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="46"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="46"/>
+    </row>
+    <row r="17" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34"/>
+      <c r="B17" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
separate storage and pad input tabs
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B019CA1D-4DE1-4642-92BA-6DEB5AB9AFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4EA8D3-95B7-47EB-8DC0-1CBEEA217E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1530" windowWidth="21840" windowHeight="13140" tabRatio="770" firstSheet="36" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="37" activeTab="42" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -54,7 +54,8 @@
     <sheet name="PipingOperationalCost" sheetId="54" r:id="rId39"/>
     <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId40"/>
     <sheet name="PadStorageCost" sheetId="70" r:id="rId41"/>
-    <sheet name="WaterQuality" sheetId="71" r:id="rId42"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -239,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="129">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -622,7 +623,10 @@
     <t>Water Quality at Production Pads (mg/L)</t>
   </si>
   <si>
-    <t>Pads and Storage</t>
+    <t>Initial Water Quality at Storage (mg/L)</t>
+  </si>
+  <si>
+    <t>Pads</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2378,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3886,7 +3890,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5855,8 +5859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FA9205-AA30-4BB4-8EBD-7F4667959AD4}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5872,7 +5876,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>125</v>
@@ -5925,6 +5929,35 @@
       <c r="B8" s="49">
         <v>188503.7</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCDA56B-EA55-4E25-9A3D-3EAA10856633}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add water component index to epsilon, other reviewer requested changes
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4EA8D3-95B7-47EB-8DC0-1CBEEA217E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D47BFE-FE3D-4701-A282-8159B8176D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="37" activeTab="42" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="5" activeTab="5" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="128">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -609,9 +609,6 @@
   </si>
   <si>
     <t>Table of Treatment Efficiency [%]</t>
-  </si>
-  <si>
-    <t>VALUE</t>
   </si>
   <si>
     <t>Table of Completions Pad Storage Capacity over Time [bbl]</t>
@@ -5806,7 +5803,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5871,15 +5868,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5940,7 +5937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCDA56B-EA55-4E25-9A3D-3EAA10856633}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5952,7 +5949,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -5989,8 +5986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6008,7 +6005,7 @@
         <v>119</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
operational model water quality calculation
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B7C44C-920B-493F-BF98-ED67F7278850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC8A1BE-CB60-491A-82CF-DFFF3407573B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="15" activeTab="17" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-1530" windowWidth="21840" windowHeight="13140" tabRatio="770" firstSheet="37" activeTab="42" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -54,6 +54,8 @@
     <sheet name="PipingOperationalCost" sheetId="54" r:id="rId39"/>
     <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId40"/>
     <sheet name="PadStorageCost" sheetId="70" r:id="rId41"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -238,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="129">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -609,17 +611,32 @@
     <t>Table of Treatment Efficiency [%]</t>
   </si>
   <si>
-    <t>VALUE</t>
-  </si>
-  <si>
     <t>Table of Completions Pad Storage Capacity over Time [bbl]</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Water Quality at Production Pads (mg/L)</t>
+  </si>
+  <si>
+    <t>Pads</t>
+  </si>
+  <si>
+    <t>Initial Water Quality at Storage (mg/L)</t>
+  </si>
+  <si>
+    <t>StorageSites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,6 +715,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -725,7 +749,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -954,12 +978,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1052,8 +1159,27 @@
     <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3035,7 +3161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19482E4D-5604-4B83-9F7A-0225AC5DE7E0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -5716,7 +5842,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5758,6 +5884,124 @@
       <c r="F3" s="45">
         <v>250</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="47">
+        <v>142277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="48">
+        <v>140998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="48">
+        <v>172490.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="48">
+        <v>257547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="48">
+        <v>241833.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="49">
+        <v>188503.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5790,7 +6034,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5808,7 +6052,7 @@
         <v>119</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add units to operational main model, add units tab to input file and run file, fix unit convert bug in results.py
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -1,61 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC8A1BE-CB60-491A-82CF-DFFF3407573B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3064B462-28F6-417E-AF16-9292CD6DA294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1530" windowWidth="21840" windowHeight="13140" tabRatio="770" firstSheet="37" activeTab="42" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" firstSheet="1" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
-    <sheet name="ProductionPads" sheetId="1" r:id="rId2"/>
-    <sheet name="ProductionTanks" sheetId="34" r:id="rId3"/>
-    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId4"/>
-    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId5"/>
-    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId6"/>
-    <sheet name="DriveDistances" sheetId="63" r:id="rId7"/>
-    <sheet name="DisposalPipeCapEx" sheetId="64" r:id="rId8"/>
-    <sheet name="CompletionsPads" sheetId="3" r:id="rId9"/>
-    <sheet name="SWDSites" sheetId="4" r:id="rId10"/>
-    <sheet name="FreshwaterSources" sheetId="35" r:id="rId11"/>
-    <sheet name="StorageSites" sheetId="36" r:id="rId12"/>
-    <sheet name="TreatmentSites" sheetId="37" r:id="rId13"/>
-    <sheet name="PRT" sheetId="59" r:id="rId14"/>
-    <sheet name="CRT" sheetId="60" r:id="rId15"/>
-    <sheet name="ReuseOptions" sheetId="38" r:id="rId16"/>
-    <sheet name="NetworkNodes" sheetId="39" r:id="rId17"/>
-    <sheet name="RCA" sheetId="67" r:id="rId18"/>
-    <sheet name="FCA" sheetId="41" r:id="rId19"/>
-    <sheet name="PCT" sheetId="42" r:id="rId20"/>
-    <sheet name="FCT" sheetId="53" r:id="rId21"/>
-    <sheet name="CCT" sheetId="57" r:id="rId22"/>
-    <sheet name="PKT" sheetId="43" r:id="rId23"/>
-    <sheet name="CKT" sheetId="44" r:id="rId24"/>
-    <sheet name="PAL" sheetId="45" r:id="rId25"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId26"/>
-    <sheet name="ProductionRates" sheetId="40" r:id="rId27"/>
-    <sheet name="PadRates" sheetId="56" r:id="rId28"/>
-    <sheet name="FlowbackRates" sheetId="58" r:id="rId29"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId30"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId31"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId32"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId33"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId34"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId35"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId36"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId37"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId38"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId39"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId40"/>
-    <sheet name="PadStorageCost" sheetId="70" r:id="rId41"/>
-    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
+    <sheet name="Units" sheetId="73" r:id="rId2"/>
+    <sheet name="ProductionPads" sheetId="1" r:id="rId3"/>
+    <sheet name="ProductionTanks" sheetId="34" r:id="rId4"/>
+    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId5"/>
+    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId6"/>
+    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId7"/>
+    <sheet name="DriveDistances" sheetId="63" r:id="rId8"/>
+    <sheet name="DisposalPipeCapEx" sheetId="64" r:id="rId9"/>
+    <sheet name="CompletionsPads" sheetId="3" r:id="rId10"/>
+    <sheet name="SWDSites" sheetId="4" r:id="rId11"/>
+    <sheet name="FreshwaterSources" sheetId="35" r:id="rId12"/>
+    <sheet name="StorageSites" sheetId="36" r:id="rId13"/>
+    <sheet name="TreatmentSites" sheetId="37" r:id="rId14"/>
+    <sheet name="PRT" sheetId="59" r:id="rId15"/>
+    <sheet name="CRT" sheetId="60" r:id="rId16"/>
+    <sheet name="ReuseOptions" sheetId="38" r:id="rId17"/>
+    <sheet name="NetworkNodes" sheetId="39" r:id="rId18"/>
+    <sheet name="RCA" sheetId="67" r:id="rId19"/>
+    <sheet name="FCA" sheetId="41" r:id="rId20"/>
+    <sheet name="PCT" sheetId="42" r:id="rId21"/>
+    <sheet name="FCT" sheetId="53" r:id="rId22"/>
+    <sheet name="CCT" sheetId="57" r:id="rId23"/>
+    <sheet name="PKT" sheetId="43" r:id="rId24"/>
+    <sheet name="CKT" sheetId="44" r:id="rId25"/>
+    <sheet name="PAL" sheetId="45" r:id="rId26"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId27"/>
+    <sheet name="ProductionRates" sheetId="40" r:id="rId28"/>
+    <sheet name="PadRates" sheetId="56" r:id="rId29"/>
+    <sheet name="FlowbackRates" sheetId="58" r:id="rId30"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId31"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId32"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId33"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId34"/>
+    <sheet name="DriveTimes" sheetId="7" r:id="rId35"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId36"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId37"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId38"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId39"/>
+    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId40"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId41"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId42"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId43"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId44"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -240,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="173">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -627,6 +628,138 @@
   </si>
   <si>
     <t>StorageSites</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>Unit Description</t>
+  </si>
+  <si>
+    <t>Unit Relationships</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>bbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume units are used to represent water flows (e.g. bbl/day), flow capacities, storage capacity, costs etc. </t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>42 gallons</t>
+  </si>
+  <si>
+    <t>kbbl</t>
+  </si>
+  <si>
+    <t>1000 bbl</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>mile</t>
+  </si>
+  <si>
+    <t>Distance units are used for defining lengths of pipelines and pipeline expansion costs</t>
+  </si>
+  <si>
+    <t>kmeter</t>
+  </si>
+  <si>
+    <t>1000 m</t>
+  </si>
+  <si>
+    <t>diameter</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>This unit applies to diameter of pipelines and pipeline expansion costs</t>
+  </si>
+  <si>
+    <t>concentration</t>
+  </si>
+  <si>
+    <t>mg/liter</t>
+  </si>
+  <si>
+    <t>Concentration unit defines water quality (e.g., TDS concentration)</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Currency unit defines costs</t>
+  </si>
+  <si>
+    <t>kUSD</t>
+  </si>
+  <si>
+    <t>1000 USD</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Time units refers to input data relative to time (e.g., water flows in bbl/day)</t>
+  </si>
+  <si>
+    <t>decision_period</t>
+  </si>
+  <si>
+    <t>decision period</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>The decision period is the amount of time in a single decision period or discretization (e.g., T01 is 1 week)</t>
+  </si>
+  <si>
+    <t>fortnight</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>30.44 days</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>kg/liter</t>
+  </si>
+  <si>
+    <t>meter</t>
   </si>
 </sst>
 </file>
@@ -723,7 +856,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,8 +881,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1060,13 +1199,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1175,6 +1428,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2100,6 +2406,184 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DB6341-94DE-401B-89F3-66EA9EB6DBB9}">
   <dimension ref="A1:R7"/>
   <sheetViews>
@@ -2228,7 +2712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABFF4F0-1521-4984-985F-ECB7FE3DE71E}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -2409,7 +2893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -2585,7 +3069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -2765,7 +3249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC3797B-8D14-4FB6-B72A-3C0C4341EC79}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2785,7 +3269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1A6821-D55E-4269-AC7B-EA9C0F0EC2AD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2805,7 +3289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -2981,7 +3465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -3157,7 +3641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19482E4D-5604-4B83-9F7A-0225AC5DE7E0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3211,7 +3695,342 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08217A32-8B76-4E4B-A189-16CA880A95B6}">
+  <sheetPr>
+    <tabColor theme="2" tint="-9.9978637043366805E-2"/>
+  </sheetPr>
+  <dimension ref="A1:AZ12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="92.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.33203125" style="1"/>
+    <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="56"/>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" s="62"/>
+      <c r="I3" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" s="63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="62"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="66"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="58"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="66"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="58"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="66"/>
+      <c r="AT8" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU8" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="AV8" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="AW8" s="67" t="s">
+        <v>149</v>
+      </c>
+      <c r="AX8" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY8" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="AZ8" s="67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="68"/>
+      <c r="I9" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="J9" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AT10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AU11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AZ11" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AU12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AZ12" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{983EC2A0-C4EA-4CE0-BED1-203B514C4F46}">
+      <formula1>$AV$9:$AV$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{EE551BFC-1380-4688-9CFB-83B42BA39880}">
+      <formula1>$AZ$9:$AZ$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{A6AF5BA9-5786-4E5D-9128-0DC2BA9560A5}">
+      <formula1>$AY$9:$AY$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{574AC30F-B080-4823-B035-087D318D4F00}">
+      <formula1>$AX$9:$AX$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{208E8586-A53E-49C9-8E44-9FD27DA62C5A}">
+      <formula1>$AW$9:$AW$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{488BC52E-41BD-40B5-A93D-07C549C24565}">
+      <formula1>$AU$9:$AU$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{6ABCC3A3-39D6-496C-BA51-98F3F4286434}">
+      <formula1>$AT$9:$AT$10</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -3296,141 +4115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
-  <dimension ref="A1:O10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="9" width="9.21875" style="1"/>
-    <col min="10" max="10" width="11.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -3512,7 +4197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3562,7 +4247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16082D3-6CFF-4538-9513-170B327E5C50}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3602,7 +4287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3685,7 +4370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3725,7 +4410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABD83BE-FC18-4B07-A835-FE113535C483}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -3921,7 +4606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -4036,12 +4721,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4455,7 +5140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -4645,7 +5330,131 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899A76A8-5CE6-4878-A6D7-FB5DF8BDAFB4}">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="9.21875" style="1"/>
+    <col min="10" max="10" width="11.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
+      <c r="C10" s="40"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -4755,7 +5564,814 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="37">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="44">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="45">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="10">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="37">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="11">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="11">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="11">
+        <v>20000</v>
+      </c>
+      <c r="F4" s="12">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>50000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.21875" style="1"/>
+    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="37"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
+        <v>2</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <v>3</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H8" s="10">
+        <v>2</v>
+      </c>
+      <c r="I8" s="37"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
+        <v>2</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="37">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="37">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="37">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="37">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="37">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="37">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="12">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
   <dimension ref="A1:R15"/>
   <sheetViews>
@@ -4937,814 +6553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="37">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="12">
-        <v>10000</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="44">
-        <v>10000</v>
-      </c>
-      <c r="C3" s="44">
-        <v>10000</v>
-      </c>
-      <c r="D3" s="44">
-        <v>10000</v>
-      </c>
-      <c r="E3" s="44">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="45">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="10">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="10">
-        <v>30000</v>
-      </c>
-      <c r="D3" s="10">
-        <v>30000</v>
-      </c>
-      <c r="E3" s="10">
-        <v>30000</v>
-      </c>
-      <c r="F3" s="37">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="11">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="11">
-        <v>20000</v>
-      </c>
-      <c r="D4" s="11">
-        <v>20000</v>
-      </c>
-      <c r="E4" s="11">
-        <v>20000</v>
-      </c>
-      <c r="F4" s="12">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="12">
-        <v>50000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.21875" style="1"/>
-    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="I3" s="37"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="H4" s="10">
-        <v>1</v>
-      </c>
-      <c r="I4" s="37">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10">
-        <v>2</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="37">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="37">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10">
-        <v>3</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="H8" s="10">
-        <v>2</v>
-      </c>
-      <c r="I8" s="37"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10">
-        <v>2</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="37"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="37"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="37"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="37">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="12">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="37">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="37">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="37">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="37">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="37">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="37">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="37">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="12">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5792,27 +6601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5826,7 +6615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -5891,7 +6680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -5972,11 +6761,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -6010,6 +6799,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59865970-D83F-46CB-8781-62CE35DBF4B5}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6029,7 +6838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -6077,7 +6886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517D4D1F-C9B2-48B7-BC2C-B9CAACD1B518}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6097,7 +6906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163385F3-A1AA-43A4-BCBF-5D7593716FB8}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6109,182 +6918,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA283BC5-D620-4970-8035-9A1157B6300D}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
correct decision period unit in input sheet, results now match main
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE6CAC4-7E60-4742-8D12-C914DC8CD123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5805892C-8331-4F57-B0EC-5072A6FD7258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1805,7 +1805,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2545,7 +2545,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3181,9 +3181,7 @@
   </sheetPr>
   <dimension ref="A1:AZ12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3395,7 +3393,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9" s="65" t="s">
         <v>145</v>
@@ -3769,7 +3767,7 @@
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
+        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="H1" s="40"/>
     </row>

</xml_diff>

<commit_message>
adjust input tab naming to match strategic model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
+++ b/pareto/case_studies/EXAMPLE_INPUT_DATA_FILE_generic_operational_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5805892C-8331-4F57-B0EC-5072A6FD7258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CECF7C-46F3-429D-816B-029DA033E579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -38,25 +38,24 @@
     <sheet name="ProductionRates" sheetId="40" r:id="rId23"/>
     <sheet name="PadRates" sheetId="56" r:id="rId24"/>
     <sheet name="FlowbackRates" sheetId="58" r:id="rId25"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId26"/>
+    <sheet name="DisposalCapacity" sheetId="46" r:id="rId26"/>
     <sheet name="TreatmentCapacity" sheetId="62" r:id="rId27"/>
     <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId28"/>
     <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId29"/>
     <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId30"/>
     <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId31"/>
     <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId32"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId33"/>
-    <sheet name="DriveDistances" sheetId="63" r:id="rId34"/>
-    <sheet name="DriveTimes" sheetId="7" r:id="rId35"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId36"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId37"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId38"/>
-    <sheet name="PipingOperationalCost" sheetId="54" r:id="rId39"/>
-    <sheet name="PadStorageCost" sheetId="70" r:id="rId40"/>
-    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId41"/>
-    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
-    <sheet name="DisposalPipeCapEx" sheetId="64" r:id="rId44"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId33"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId34"/>
+    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId35"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId36"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId37"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId38"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId39"/>
+    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId40"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId41"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId42"/>
+    <sheet name="DisposalPipeCapEx" sheetId="64" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -241,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="154">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -703,9 +702,6 @@
   </si>
   <si>
     <t>meter</t>
-  </si>
-  <si>
-    <t>Table of Drive Times between Sites</t>
   </si>
 </sst>
 </file>
@@ -3751,6 +3747,9 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5119,6 +5118,242 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Reuse Operational Cost [USD/bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Piping Operational Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Piping Operational Costs [USD/bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity over Time [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Completions Pad Storage Capacity over Time [bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="44">
+        <v>250</v>
+      </c>
+      <c r="C3" s="44">
+        <v>250</v>
+      </c>
+      <c r="D3" s="44">
+        <v>250</v>
+      </c>
+      <c r="E3" s="44">
+        <v>250</v>
+      </c>
+      <c r="F3" s="45">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -5218,30 +5453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517D4D1F-C9B2-48B7-BC2C-B9CAACD1B518}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -5503,173 +5715,6 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Reuse Operational Cost [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Piping Operational Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Piping Operational Costs [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0.85</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5863,75 +5908,6 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity over Time [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Completions Pad Storage Capacity over Time [bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="44">
-        <v>250</v>
-      </c>
-      <c r="C3" s="44">
-        <v>250</v>
-      </c>
-      <c r="D3" s="44">
-        <v>250</v>
-      </c>
-      <c r="E3" s="44">
-        <v>250</v>
-      </c>
-      <c r="F3" s="45">
-        <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -5982,7 +5958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -6067,7 +6043,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -6108,7 +6084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163385F3-A1AA-43A4-BCBF-5D7593716FB8}">
   <sheetPr>
     <tabColor theme="5"/>

</xml_diff>